<commit_message>
Added Correct.Response column to lists
</commit_message>
<xml_diff>
--- a/writeups/projects/fellowship conference 2022/figures/excel_visuals/Poster 07.31 Figures.xlsx
+++ b/writeups/projects/fellowship conference 2022/figures/excel_visuals/Poster 07.31 Figures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\Projects\Fellowship Conference 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\SI.SP\writeups\projects\fellowship conference 2022\figures\excel_visuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9F6B4D-4245-458D-A2C9-AB1D90860569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BCD144-C455-461B-8A80-F097F25DCCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BE94E350-9BA2-40B7-B37A-9E00105A1A32}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>Personal</t>
   </si>
   <si>
-    <t>Penninsula</t>
-  </si>
-  <si>
     <t>Parasite</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>Talker B</t>
+  </si>
+  <si>
+    <t>Peninsula</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -655,18 +655,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,9 +733,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -753,7 +752,61 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -767,60 +820,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26893740-08BF-46AB-82EB-D9B605E89688}">
   <dimension ref="B2:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19:U31"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1178,560 +1177,556 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D2" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="D2" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="2:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="H3" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="57" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="72"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="2:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="59"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="28" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="48"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="30" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="42"/>
+      <c r="F5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="49"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="65"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-    </row>
-    <row r="6" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="59"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="63"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="69"/>
       <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="19" t="s">
+      <c r="K6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="17" t="s">
-        <v>22</v>
+      <c r="N6" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="59"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="63"/>
-      <c r="J7" s="25" t="s">
+      <c r="E7" s="42"/>
+      <c r="F7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="69"/>
+      <c r="J7" s="24" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="59"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="26" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="63"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="49"/>
+      <c r="H8" s="69"/>
       <c r="J8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="19" t="s">
+      <c r="K8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="17" t="s">
-        <v>38</v>
+      <c r="N8" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="59"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="63"/>
-      <c r="J9" s="25" t="s">
+      <c r="E9" s="42"/>
+      <c r="F9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="49"/>
+      <c r="H9" s="69"/>
+      <c r="J9" s="24" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="21" t="s">
-        <v>20</v>
+      <c r="N9" s="20" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="59"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="26" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="63"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="49"/>
+      <c r="H10" s="69"/>
       <c r="J10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>26</v>
+      <c r="N10" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="59"/>
-      <c r="C11" s="46"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="63"/>
-      <c r="J11" s="25" t="s">
+      <c r="E11" s="42"/>
+      <c r="F11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="69"/>
+      <c r="J11" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="21" t="s">
-        <v>34</v>
+      <c r="N11" s="20" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="59"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="26" t="s">
+      <c r="B12" s="65"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="50"/>
-      <c r="H12" s="63"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="49"/>
+      <c r="H12" s="69"/>
       <c r="J12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="M12" s="19" t="s">
+      <c r="K12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="17" t="s">
-        <v>32</v>
+      <c r="N12" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="59"/>
-      <c r="C13" s="46"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="50"/>
-      <c r="H13" s="63"/>
-      <c r="J13" s="25" t="s">
+      <c r="E13" s="41"/>
+      <c r="F13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="49"/>
+      <c r="H13" s="69"/>
+      <c r="J13" s="24" t="s">
         <v>10</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N13" s="21" t="s">
-        <v>30</v>
+      <c r="N13" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="59"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="63"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="69"/>
       <c r="J14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="M14" s="22" t="s">
+      <c r="K14" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="65"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="69"/>
+    </row>
+    <row r="16" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="65"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="69"/>
+    </row>
+    <row r="17" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="65"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="49"/>
+      <c r="H17" s="69"/>
+    </row>
+    <row r="18" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="65"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="59"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="63"/>
-    </row>
-    <row r="16" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="59"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="63"/>
-    </row>
-    <row r="17" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="59"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="63"/>
-    </row>
-    <row r="18" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="59"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="50"/>
-      <c r="H18" s="63"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="69"/>
     </row>
     <row r="19" spans="2:34" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="59"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="21" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="50"/>
-      <c r="H19" s="63"/>
-      <c r="P19" s="67" t="s">
+      <c r="G19" s="49"/>
+      <c r="H19" s="69"/>
+      <c r="P19" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="Q19" s="67"/>
-      <c r="R19" s="66"/>
-      <c r="S19" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="T19" s="67"/>
+      <c r="T19" s="70"/>
     </row>
     <row r="20" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="59"/>
-      <c r="C20" s="46"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="34"/>
+      <c r="F20" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="50"/>
-      <c r="H20" s="63"/>
-      <c r="P20" s="68" t="s">
+      <c r="G20" s="49"/>
+      <c r="H20" s="69"/>
+      <c r="P20" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="Q20" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="R20" s="66"/>
-      <c r="S20" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="T20" s="73" t="s">
+      <c r="R20" s="55"/>
+      <c r="S20" s="60" t="s">
         <v>44</v>
       </c>
+      <c r="T20" s="61" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="21" spans="2:34" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="59"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="26" t="s">
+      <c r="B21" s="65"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="21" t="s">
+      <c r="E21" s="34"/>
+      <c r="F21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="50"/>
-      <c r="H21" s="63"/>
-      <c r="P21" s="70" t="s">
+      <c r="G21" s="49"/>
+      <c r="H21" s="69"/>
+      <c r="P21" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q21" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q21" s="71" t="s">
+      <c r="R21" s="55"/>
+      <c r="S21" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="T21" s="63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="65"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="34"/>
+      <c r="F22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="49"/>
+      <c r="H22" s="69"/>
+      <c r="P22" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q22" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R21" s="66"/>
-      <c r="S21" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="T21" s="75" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="59"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="4" t="s">
+    </row>
+    <row r="23" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="65"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="50"/>
-      <c r="H22" s="63"/>
-      <c r="P22" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q22" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="59"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="21" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="50"/>
-      <c r="H23" s="63"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="69"/>
       <c r="P23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="Q23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="T23" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="65"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="49"/>
+      <c r="H24" s="69"/>
+      <c r="P24" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="S23" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="T23" s="26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="59"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="63"/>
-      <c r="P24" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q24" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>43</v>
+      <c r="S24" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:34" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="59"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="23" t="s">
+      <c r="B25" s="65"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="51"/>
-      <c r="H25" s="63"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="69"/>
       <c r="P25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q25" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="S25" s="19" t="s">
+      <c r="Q25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="T25" s="26" t="s">
-        <v>25</v>
+      <c r="T25" s="25" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="59"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="63"/>
-      <c r="P26" s="25" t="s">
+      <c r="B26" s="65"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="37"/>
+      <c r="H26" s="69"/>
+      <c r="P26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="Q26" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S26" s="16" t="s">
+      <c r="Q26" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="S26" s="15" t="s">
         <v>5</v>
       </c>
       <c r="T26" s="4" t="s">
@@ -1739,93 +1734,93 @@
       </c>
     </row>
     <row r="27" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
+      <c r="D27" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
       <c r="P27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="17" t="s">
+      <c r="Q27" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="S27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="T27" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P28" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q28" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="S28" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="T28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S27" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="T27" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="P28" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q28" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="S28" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="T28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF28" s="11"/>
-      <c r="AG28" s="11"/>
-      <c r="AH28" s="11"/>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="10"/>
+      <c r="AH28" s="10"/>
     </row>
     <row r="29" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q29" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="S29" s="19" t="s">
+      <c r="Q29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="T29" s="26" t="s">
-        <v>28</v>
+      <c r="T29" s="25" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="P30" s="25" t="s">
+      <c r="P30" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="Q30" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="S30" s="16" t="s">
+      <c r="Q30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="S30" s="15" t="s">
         <v>1</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="2:34" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q31" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="S31" s="22" t="s">
+      <c r="Q31" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="S31" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="T31" s="27" t="s">
-        <v>33</v>
+      <c r="T31" s="26" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="S19:T19"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="B3:B26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="H3:H26"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="S19:T19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>